<commit_message>
parser now goes vroom
</commit_message>
<xml_diff>
--- a/TestDocuments/Timings.xlsx
+++ b/TestDocuments/Timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Prosetta\TestDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0C7EF9C-6CAD-4894-803B-0BAE764E7771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767B05EE-1C4F-4D42-85AA-80671D2ABD36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" xr2:uid="{0B891BD4-AF55-49BB-B4E5-3B15BB25AD0E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Debug</t>
   </si>
@@ -54,18 +53,41 @@
     <t>Version</t>
   </si>
   <si>
-    <t>Seconds</t>
-  </si>
-  <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Time Per Step</t>
+  </si>
+  <si>
+    <t>Sec1</t>
+  </si>
+  <si>
+    <t>Sec2</t>
+  </si>
+  <si>
+    <t>Sec3</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Frac</t>
+  </si>
+  <si>
+    <t>Cache NE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="175" formatCode="0.0000000"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -96,12 +118,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,30 +460,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7891AC-DEEF-43B1-ADEC-B5C7AEDE7970}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="10.80859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.76171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -469,12 +517,20 @@
       <c r="C2">
         <v>179</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f>TEXT(C2/(24*60*60),"hh:mm:ss")</f>
+      <c r="F2" s="4">
+        <f t="shared" ref="F2:F4" si="0">AVERAGE(C2:E2)</f>
+        <v>179</v>
+      </c>
+      <c r="G2" s="3">
+        <f>F2/86400</f>
+        <v>2.0717592592592593E-3</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>TEXT(G2,"hh:mm:ss")</f>
         <v>00:02:59</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -482,14 +538,31 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>120</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>TEXT(C3/(24*60*60),"hh:mm:ss")</f>
-        <v>00:02:00</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <v>146</v>
+      </c>
+      <c r="E3">
+        <v>136</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G7" si="1">F3/86400</f>
+        <v>1.6435185185185185E-3</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f t="shared" ref="H3:H7" si="2">TEXT(G3,"hh:mm:ss")</f>
+        <v>00:02:22</v>
+      </c>
+      <c r="I3">
+        <v>1658103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -499,12 +572,20 @@
       <c r="C4">
         <v>151</v>
       </c>
-      <c r="D4" s="1" t="str">
-        <f>TEXT(C4/(24*60*60),"hh:mm:ss")</f>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.7476851851851852E-3</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00:02:31</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -512,12 +593,96 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f>TEXT(C5/(24*60*60),"hh:mm:ss")</f>
-        <v>00:01:48</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D5">
+        <v>99</v>
+      </c>
+      <c r="E5">
+        <v>104</v>
+      </c>
+      <c r="F5" s="4">
+        <f>AVERAGE(C5:E5)</f>
+        <v>101.33333333333333</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
+        <v>1.1728395061728395E-3</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00:01:41</v>
+      </c>
+      <c r="I5">
+        <v>1488535</v>
+      </c>
+      <c r="J5" s="3">
+        <f>C5/I5</f>
+        <v>6.785194839221113E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" ref="F6:F7" si="3">AVERAGE(C6:E6)</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00:00:03</v>
+      </c>
+      <c r="I6">
+        <v>45277</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="1"/>
+        <v>3.4722222222222222E-5</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00:00:03</v>
+      </c>
+      <c r="I7">
+        <v>45277</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="G8" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>